<commit_message>
tests: pincher + enhanced gemini error handling
</commit_message>
<xml_diff>
--- a/generated-tests/pincher/frontend/direct/metrics.xlsx
+++ b/generated-tests/pincher/frontend/direct/metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marius\Desktop\Bachelor-Arbeit\test-generation-app\generated-tests\pincher\frontend\direct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543D3F82-8403-4951-9D1B-0E41B6F7F15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC44A902-91CF-4595-8DB6-3EACBFF618D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{73C55193-3CB0-42EF-A4B9-F7B9A2E05BE9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73C55193-3CB0-42EF-A4B9-F7B9A2E05BE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Test</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>reports-2.spec</t>
+  </si>
+  <si>
+    <t>person-1.spec</t>
+  </si>
+  <si>
+    <t>persons</t>
+  </si>
+  <si>
+    <t>overview (person)</t>
+  </si>
+  <si>
+    <t>base (person)</t>
+  </si>
+  <si>
+    <t>person</t>
   </si>
 </sst>
 </file>
@@ -362,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -395,6 +410,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -736,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE60AEF-AC79-4BE5-B0FB-2A2449C95BDE}">
   <dimension ref="D5:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,47 +869,89 @@
       <c r="M8" s="31"/>
     </row>
     <row r="9" spans="4:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D9" s="11"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="D9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="21">
+        <v>23</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="22">
+        <v>33</v>
+      </c>
+      <c r="I9" s="6">
+        <v>4</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1</v>
+      </c>
+      <c r="K9" s="6">
+        <v>11</v>
+      </c>
+      <c r="L9" s="6">
+        <v>15</v>
+      </c>
       <c r="M9" s="6"/>
     </row>
     <row r="10" spans="4:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D10" s="12"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="19">
+        <v>100</v>
+      </c>
+      <c r="G10" s="32">
+        <v>100</v>
+      </c>
+      <c r="H10" s="20">
+        <v>100</v>
+      </c>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="4:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D11" s="10"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="E11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="32">
+        <v>38</v>
+      </c>
+      <c r="G11" s="32">
+        <v>12</v>
+      </c>
+      <c r="H11" s="20">
+        <v>49</v>
+      </c>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="4:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D12" s="10"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="20"/>
+      <c r="E12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="19">
+        <v>0</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0</v>
+      </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>

</xml_diff>